<commit_message>
suite commit propre, les fichiers de William sont dans le projet
</commit_message>
<xml_diff>
--- a/RAW1/Soil_analysis.xlsx
+++ b/RAW1/Soil_analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumniumonsac-my.sharepoint.com/personal/151201_umons_ac_be/Documents/UMONS/MA2/MEMOIRE/Statistique/R/MEMOIRE/RAW1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumniumonsac-my.sharepoint.com/personal/151201_umons_ac_be/Documents/UMONS/MA2/MEMOIRE/Statistique/R/STAT-MEMOIRE/RAW1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="8_{B97CC621-0325-4EBD-B490-53D71178061E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1CFE0AB-5BA8-49DF-8FE7-F6110518B7CE}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="8_{B97CC621-0325-4EBD-B490-53D71178061E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54F71094-4676-4325-9695-73267CD4F071}"/>
   <bookViews>
-    <workbookView xWindow="34950" yWindow="1230" windowWidth="21600" windowHeight="11385" tabRatio="704" activeTab="5" xr2:uid="{64FE5FAE-006E-7340-805C-05441D62BA48}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="704" activeTab="6" xr2:uid="{64FE5FAE-006E-7340-805C-05441D62BA48}"/>
   </bookViews>
   <sheets>
     <sheet name="Résultats nitrates" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="109">
   <si>
     <t>Abbaye Saint Denis</t>
   </si>
@@ -323,6 +323,51 @@
   </si>
   <si>
     <t>Parc Bonaert</t>
+  </si>
+  <si>
+    <t>Site 1</t>
+  </si>
+  <si>
+    <t>Site 2</t>
+  </si>
+  <si>
+    <t>Site 3</t>
+  </si>
+  <si>
+    <t>Site 4</t>
+  </si>
+  <si>
+    <t>Site 5</t>
+  </si>
+  <si>
+    <t>Site 6</t>
+  </si>
+  <si>
+    <t>Site 7</t>
+  </si>
+  <si>
+    <t>Site 8</t>
+  </si>
+  <si>
+    <t>Site 9</t>
+  </si>
+  <si>
+    <t>Site 10</t>
+  </si>
+  <si>
+    <t>Site 11</t>
+  </si>
+  <si>
+    <t>Site 12</t>
+  </si>
+  <si>
+    <t>Site 13</t>
+  </si>
+  <si>
+    <t>Site 14</t>
+  </si>
+  <si>
+    <t>Site 15</t>
   </si>
 </sst>
 </file>
@@ -334,7 +379,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -358,6 +403,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -980,27 +1031,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1011,6 +1041,27 @@
     <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1029,7 +1080,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1331,7 +1382,7 @@
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="25.5" customWidth="1"/>
     <col min="2" max="2" width="15.125" customWidth="1"/>
@@ -1795,7 +1846,7 @@
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="25.5" customWidth="1"/>
     <col min="2" max="2" width="17.625" customWidth="1"/>
@@ -2138,10 +2189,10 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="25.5" customWidth="1"/>
     <col min="2" max="2" width="24.375" customWidth="1"/>
@@ -2629,10 +2680,10 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="25.375" customWidth="1"/>
     <col min="2" max="2" width="19.875" customWidth="1"/>
@@ -2792,7 +2843,7 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="3" width="25.5" customWidth="1"/>
     <col min="4" max="4" width="25.375" customWidth="1"/>
@@ -3966,12 +4017,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F20FFBF9-F8A9-47AF-A143-F1280D1DFEC4}">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+    <sheetView zoomScale="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="25.375" customWidth="1"/>
     <col min="2" max="2" width="25.625" customWidth="1"/>
@@ -4034,28 +4085,28 @@
       <c r="S1" s="116"/>
     </row>
     <row r="2" spans="1:19">
-      <c r="A2" s="125" t="s">
+      <c r="A2" s="118" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="126">
+      <c r="B2" s="119">
         <v>6.27</v>
       </c>
-      <c r="C2" s="126">
+      <c r="C2" s="119">
         <v>0.46</v>
       </c>
-      <c r="D2" s="127">
+      <c r="D2" s="120">
         <v>36.200000000000003</v>
       </c>
-      <c r="E2" s="127">
+      <c r="E2" s="120">
         <v>29.5</v>
       </c>
-      <c r="F2" s="128">
+      <c r="F2" s="121">
         <v>0.12</v>
       </c>
-      <c r="G2" s="127">
+      <c r="G2" s="120">
         <v>13.7</v>
       </c>
-      <c r="H2" s="127">
+      <c r="H2" s="120">
         <v>89.6</v>
       </c>
       <c r="I2" s="109">
@@ -4075,28 +4126,28 @@
       <c r="O2" s="38"/>
     </row>
     <row r="3" spans="1:19">
-      <c r="A3" s="125" t="s">
+      <c r="A3" s="118" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="126">
+      <c r="B3" s="119">
         <v>6.33</v>
       </c>
-      <c r="C3" s="126">
+      <c r="C3" s="119">
         <v>0.64</v>
       </c>
-      <c r="D3" s="127">
+      <c r="D3" s="120">
         <v>39.6</v>
       </c>
-      <c r="E3" s="127">
+      <c r="E3" s="120">
         <v>20.7</v>
       </c>
-      <c r="F3" s="128">
+      <c r="F3" s="121">
         <v>0.08</v>
       </c>
-      <c r="G3" s="127">
+      <c r="G3" s="120">
         <v>16.5</v>
       </c>
-      <c r="H3" s="127">
+      <c r="H3" s="120">
         <v>34.1</v>
       </c>
       <c r="I3" s="74">
@@ -4116,28 +4167,28 @@
       <c r="O3" s="38"/>
     </row>
     <row r="4" spans="1:19">
-      <c r="A4" s="125" t="s">
+      <c r="A4" s="118" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="126">
+      <c r="B4" s="119">
         <v>6.97</v>
       </c>
-      <c r="C4" s="128">
+      <c r="C4" s="121">
         <v>0.4</v>
       </c>
-      <c r="D4" s="127">
+      <c r="D4" s="120">
         <v>28</v>
       </c>
-      <c r="E4" s="127">
+      <c r="E4" s="120">
         <v>24.8</v>
       </c>
-      <c r="F4" s="129">
+      <c r="F4" s="122">
         <v>0.21</v>
       </c>
-      <c r="G4" s="126">
+      <c r="G4" s="119">
         <v>6.69</v>
       </c>
-      <c r="H4" s="130">
+      <c r="H4" s="123">
         <v>135</v>
       </c>
       <c r="I4" s="109">
@@ -4157,28 +4208,28 @@
       <c r="O4" s="39"/>
     </row>
     <row r="5" spans="1:19">
-      <c r="A5" s="125" t="s">
+      <c r="A5" s="118" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="126">
+      <c r="B5" s="119">
         <v>7.91</v>
       </c>
-      <c r="C5" s="128">
+      <c r="C5" s="121">
         <v>0.72</v>
       </c>
-      <c r="D5" s="131">
+      <c r="D5" s="124">
         <v>66.7</v>
       </c>
-      <c r="E5" s="127">
+      <c r="E5" s="120">
         <v>25</v>
       </c>
-      <c r="F5" s="129">
+      <c r="F5" s="122">
         <v>0.33500000000000002</v>
       </c>
-      <c r="G5" s="127">
+      <c r="G5" s="120">
         <v>15.8</v>
       </c>
-      <c r="H5" s="127">
+      <c r="H5" s="120">
         <v>72.099999999999994</v>
       </c>
       <c r="I5" s="74">
@@ -4198,28 +4249,28 @@
       <c r="O5" s="38"/>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="125" t="s">
+      <c r="A6" s="118" t="s">
         <v>87</v>
       </c>
-      <c r="B6" s="126">
+      <c r="B6" s="119">
         <v>3.18</v>
       </c>
-      <c r="C6" s="128">
+      <c r="C6" s="121">
         <v>0.38</v>
       </c>
-      <c r="D6" s="127">
+      <c r="D6" s="120">
         <v>24.1</v>
       </c>
-      <c r="E6" s="127">
+      <c r="E6" s="120">
         <v>15.4</v>
       </c>
-      <c r="F6" s="128">
+      <c r="F6" s="121">
         <v>0.27600000000000002</v>
       </c>
-      <c r="G6" s="126">
+      <c r="G6" s="119">
         <v>4.79</v>
       </c>
-      <c r="H6" s="127">
+      <c r="H6" s="120">
         <v>58.7</v>
       </c>
       <c r="I6" s="74">
@@ -4239,28 +4290,28 @@
       <c r="O6" s="38"/>
     </row>
     <row r="7" spans="1:19">
-      <c r="A7" s="125" t="s">
+      <c r="A7" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="126">
+      <c r="B7" s="119">
         <v>8.14</v>
       </c>
-      <c r="C7" s="128">
+      <c r="C7" s="121">
         <v>0.56999999999999995</v>
       </c>
-      <c r="D7" s="127">
+      <c r="D7" s="120">
         <v>34.200000000000003</v>
       </c>
-      <c r="E7" s="131">
+      <c r="E7" s="124">
         <v>96.2</v>
       </c>
-      <c r="F7" s="132">
+      <c r="F7" s="125">
         <v>1.5489999999999999</v>
       </c>
-      <c r="G7" s="127">
+      <c r="G7" s="120">
         <v>19.3</v>
       </c>
-      <c r="H7" s="133">
+      <c r="H7" s="126">
         <v>412</v>
       </c>
       <c r="I7" s="109">
@@ -4280,28 +4331,28 @@
       <c r="O7" s="39"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="A8" s="125" t="s">
+      <c r="A8" s="118" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="126">
+      <c r="B8" s="119">
         <v>6.06</v>
       </c>
-      <c r="C8" s="126">
+      <c r="C8" s="119">
         <v>0.16</v>
       </c>
-      <c r="D8" s="127">
+      <c r="D8" s="120">
         <v>26.2</v>
       </c>
-      <c r="E8" s="126">
+      <c r="E8" s="119">
         <v>8.56</v>
       </c>
-      <c r="F8" s="128">
+      <c r="F8" s="121">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G8" s="126">
+      <c r="G8" s="119">
         <v>7.2</v>
       </c>
-      <c r="H8" s="127">
+      <c r="H8" s="120">
         <v>27.2</v>
       </c>
       <c r="I8" s="74">
@@ -4321,28 +4372,28 @@
       <c r="O8" s="38"/>
     </row>
     <row r="9" spans="1:19">
-      <c r="A9" s="125" t="s">
+      <c r="A9" s="118" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="126">
+      <c r="B9" s="119">
         <v>7.87</v>
       </c>
-      <c r="C9" s="128">
+      <c r="C9" s="121">
         <v>0.68</v>
       </c>
-      <c r="D9" s="127">
+      <c r="D9" s="120">
         <v>41.4</v>
       </c>
-      <c r="E9" s="127">
+      <c r="E9" s="120">
         <v>29.4</v>
       </c>
-      <c r="F9" s="129">
+      <c r="F9" s="122">
         <v>0.17399999999999999</v>
       </c>
-      <c r="G9" s="126">
+      <c r="G9" s="119">
         <v>20</v>
       </c>
-      <c r="H9" s="127">
+      <c r="H9" s="120">
         <v>62.8</v>
       </c>
       <c r="I9" s="74">
@@ -4362,28 +4413,28 @@
       <c r="O9" s="38"/>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="125" t="s">
+      <c r="A10" s="118" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="126">
+      <c r="B10" s="119">
         <v>6.44</v>
       </c>
-      <c r="C10" s="126">
+      <c r="C10" s="119">
         <v>0.39</v>
       </c>
-      <c r="D10" s="127">
+      <c r="D10" s="120">
         <v>32.6</v>
       </c>
-      <c r="E10" s="127">
+      <c r="E10" s="120">
         <v>31.3</v>
       </c>
-      <c r="F10" s="128">
+      <c r="F10" s="121">
         <v>0.13</v>
       </c>
-      <c r="G10" s="127">
+      <c r="G10" s="120">
         <v>16.2</v>
       </c>
-      <c r="H10" s="127">
+      <c r="H10" s="120">
         <v>89.6</v>
       </c>
       <c r="I10" s="109">
@@ -4403,28 +4454,28 @@
       <c r="O10" s="38"/>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="125" t="s">
+      <c r="A11" s="118" t="s">
         <v>89</v>
       </c>
-      <c r="B11" s="127">
+      <c r="B11" s="120">
         <v>11.2</v>
       </c>
-      <c r="C11" s="128">
+      <c r="C11" s="121">
         <v>0.92</v>
       </c>
-      <c r="D11" s="127">
+      <c r="D11" s="120">
         <v>42.3</v>
       </c>
-      <c r="E11" s="127">
+      <c r="E11" s="120">
         <v>33.799999999999997</v>
       </c>
-      <c r="F11" s="129">
+      <c r="F11" s="122">
         <v>0.33100000000000002</v>
       </c>
-      <c r="G11" s="127">
+      <c r="G11" s="120">
         <v>25.6</v>
       </c>
-      <c r="H11" s="127">
+      <c r="H11" s="120">
         <v>84.9</v>
       </c>
       <c r="I11" s="109">
@@ -4444,28 +4495,28 @@
       <c r="O11" s="38"/>
     </row>
     <row r="12" spans="1:19">
-      <c r="A12" s="125" t="s">
+      <c r="A12" s="118" t="s">
         <v>90</v>
       </c>
-      <c r="B12" s="127">
+      <c r="B12" s="120">
         <v>11.4</v>
       </c>
-      <c r="C12" s="126">
+      <c r="C12" s="119">
         <v>0.68</v>
       </c>
-      <c r="D12" s="127">
+      <c r="D12" s="120">
         <v>49.9</v>
       </c>
-      <c r="E12" s="134">
+      <c r="E12" s="127">
         <v>103</v>
       </c>
-      <c r="F12" s="128">
+      <c r="F12" s="121">
         <v>0.37</v>
       </c>
-      <c r="G12" s="127">
+      <c r="G12" s="120">
         <v>24.6</v>
       </c>
-      <c r="H12" s="133">
+      <c r="H12" s="126">
         <v>491</v>
       </c>
       <c r="I12" s="110">
@@ -4485,28 +4536,28 @@
       <c r="O12" s="39"/>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" s="125" t="s">
+      <c r="A13" s="118" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="126">
+      <c r="B13" s="119">
         <v>8.3800000000000008</v>
       </c>
-      <c r="C13" s="128">
+      <c r="C13" s="121">
         <v>0.67</v>
       </c>
-      <c r="D13" s="127">
+      <c r="D13" s="120">
         <v>45.8</v>
       </c>
-      <c r="E13" s="127">
+      <c r="E13" s="120">
         <v>25.7</v>
       </c>
-      <c r="F13" s="129">
+      <c r="F13" s="122">
         <v>0.27800000000000002</v>
       </c>
-      <c r="G13" s="127">
+      <c r="G13" s="120">
         <v>23.1</v>
       </c>
-      <c r="H13" s="127">
+      <c r="H13" s="120">
         <v>93.5</v>
       </c>
       <c r="I13" s="109">
@@ -4526,28 +4577,28 @@
       <c r="O13" s="38"/>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" s="125" t="s">
+      <c r="A14" s="118" t="s">
         <v>91</v>
       </c>
-      <c r="B14" s="126">
+      <c r="B14" s="119">
         <v>5.8</v>
       </c>
-      <c r="C14" s="128">
+      <c r="C14" s="121">
         <v>0.47</v>
       </c>
-      <c r="D14" s="127">
+      <c r="D14" s="120">
         <v>40.700000000000003</v>
       </c>
-      <c r="E14" s="127">
+      <c r="E14" s="120">
         <v>43.6</v>
       </c>
-      <c r="F14" s="129">
+      <c r="F14" s="122">
         <v>0.51800000000000002</v>
       </c>
-      <c r="G14" s="127">
+      <c r="G14" s="120">
         <v>13.6</v>
       </c>
-      <c r="H14" s="130">
+      <c r="H14" s="123">
         <v>128</v>
       </c>
       <c r="I14" s="109">
@@ -4567,28 +4618,28 @@
       <c r="O14" s="39"/>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="125" t="s">
+      <c r="A15" s="118" t="s">
         <v>92</v>
       </c>
-      <c r="B15" s="126">
+      <c r="B15" s="119">
         <v>7.46</v>
       </c>
-      <c r="C15" s="128">
+      <c r="C15" s="121">
         <v>0.46</v>
       </c>
-      <c r="D15" s="127">
+      <c r="D15" s="120">
         <v>38.6</v>
       </c>
-      <c r="E15" s="127">
+      <c r="E15" s="120">
         <v>18.7</v>
       </c>
-      <c r="F15" s="128">
+      <c r="F15" s="121">
         <v>0.12</v>
       </c>
-      <c r="G15" s="127">
+      <c r="G15" s="120">
         <v>20.6</v>
       </c>
-      <c r="H15" s="127">
+      <c r="H15" s="120">
         <v>39.700000000000003</v>
       </c>
       <c r="I15" s="74">
@@ -4608,7 +4659,7 @@
       <c r="O15" s="38"/>
     </row>
     <row r="16" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A16" s="125" t="s">
+      <c r="A16" s="118" t="s">
         <v>93</v>
       </c>
       <c r="B16" s="111">
@@ -5076,1429 +5127,1475 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24676B4F-79F9-084F-BF50-2899E1D4D67F}">
-  <dimension ref="A1:P33"/>
+  <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView zoomScale="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="25.375" customWidth="1"/>
-    <col min="2" max="2" width="25.625" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="27.375" customWidth="1"/>
-    <col min="5" max="5" width="26.875" customWidth="1"/>
-    <col min="6" max="6" width="24.875" customWidth="1"/>
-    <col min="7" max="7" width="28.375" customWidth="1"/>
-    <col min="8" max="8" width="26.5" customWidth="1"/>
-    <col min="9" max="12" width="25.875" customWidth="1"/>
-    <col min="13" max="13" width="25.375" customWidth="1"/>
-    <col min="14" max="14" width="24.625" customWidth="1"/>
-    <col min="15" max="15" width="26.875" customWidth="1"/>
-    <col min="16" max="16" width="21.625" customWidth="1"/>
+    <col min="2" max="2" width="25.375" customWidth="1"/>
+    <col min="3" max="3" width="25.625" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="27.375" customWidth="1"/>
+    <col min="6" max="6" width="26.875" customWidth="1"/>
+    <col min="7" max="7" width="24.875" customWidth="1"/>
+    <col min="8" max="8" width="28.375" customWidth="1"/>
+    <col min="9" max="9" width="26.5" customWidth="1"/>
+    <col min="10" max="13" width="25.875" customWidth="1"/>
+    <col min="14" max="14" width="25.375" customWidth="1"/>
+    <col min="15" max="15" width="24.625" customWidth="1"/>
+    <col min="16" max="16" width="26.875" customWidth="1"/>
+    <col min="17" max="17" width="21.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="97" customFormat="1">
-      <c r="A1" s="121" t="s">
+    <row r="1" spans="1:17" s="97" customFormat="1">
+      <c r="B1" s="128" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="121" t="s">
+      <c r="C1" s="129"/>
+      <c r="D1" s="128" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="122"/>
-      <c r="E1" s="121" t="s">
+      <c r="E1" s="129"/>
+      <c r="F1" s="128" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="122"/>
-      <c r="G1" s="121" t="s">
+      <c r="G1" s="129"/>
+      <c r="H1" s="128" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="122"/>
-      <c r="I1" s="121" t="s">
+      <c r="I1" s="129"/>
+      <c r="J1" s="128" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="122"/>
-      <c r="K1" s="121" t="s">
+      <c r="K1" s="129"/>
+      <c r="L1" s="128" t="s">
         <v>33</v>
       </c>
-      <c r="L1" s="122"/>
-      <c r="M1" s="121" t="s">
+      <c r="M1" s="129"/>
+      <c r="N1" s="128" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="122"/>
-      <c r="O1" s="121" t="s">
+      <c r="O1" s="129"/>
+      <c r="P1" s="128" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="122"/>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="8" t="s">
+      <c r="Q1" s="129"/>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="21">
+      <c r="C2" s="21">
         <v>6.27</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="21">
+      <c r="D2" s="40"/>
+      <c r="E2" s="21">
         <v>0.46</v>
       </c>
-      <c r="E2" s="40"/>
-      <c r="F2" s="17">
+      <c r="F2" s="40"/>
+      <c r="G2" s="17">
         <v>36.200000000000003</v>
       </c>
-      <c r="G2" s="38"/>
-      <c r="H2" s="17">
+      <c r="H2" s="38"/>
+      <c r="I2" s="17">
         <v>29.5</v>
       </c>
-      <c r="I2" s="38"/>
-      <c r="J2" s="23">
+      <c r="J2" s="38"/>
+      <c r="K2" s="23">
         <v>0.12</v>
       </c>
-      <c r="K2" s="42"/>
-      <c r="L2" s="17">
+      <c r="L2" s="42"/>
+      <c r="M2" s="17">
         <v>13.7</v>
       </c>
-      <c r="M2" s="38"/>
-      <c r="N2" s="17">
+      <c r="N2" s="38"/>
+      <c r="O2" s="17">
         <v>89.6</v>
       </c>
-      <c r="O2" s="38"/>
-      <c r="P2" s="26">
+      <c r="P2" s="38"/>
+      <c r="Q2" s="26">
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:17">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="21">
+      <c r="C3" s="21">
         <v>6.33</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="21">
+      <c r="D3" s="40"/>
+      <c r="E3" s="21">
         <v>0.64</v>
       </c>
-      <c r="E3" s="40"/>
-      <c r="F3" s="17">
+      <c r="F3" s="40"/>
+      <c r="G3" s="17">
         <v>39.6</v>
       </c>
-      <c r="G3" s="38"/>
-      <c r="H3" s="17">
+      <c r="H3" s="38"/>
+      <c r="I3" s="17">
         <v>20.7</v>
       </c>
-      <c r="I3" s="38"/>
-      <c r="J3" s="23">
+      <c r="J3" s="38"/>
+      <c r="K3" s="23">
         <v>0.08</v>
       </c>
-      <c r="K3" s="42"/>
-      <c r="L3" s="17">
+      <c r="L3" s="42"/>
+      <c r="M3" s="17">
         <v>16.5</v>
       </c>
-      <c r="M3" s="38"/>
-      <c r="N3" s="17">
+      <c r="N3" s="38"/>
+      <c r="O3" s="17">
         <v>34.1</v>
       </c>
-      <c r="O3" s="38"/>
-      <c r="P3" s="18">
+      <c r="P3" s="38"/>
+      <c r="Q3" s="18">
         <v>93.2</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:17">
+      <c r="A4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="21">
+      <c r="C4" s="21">
         <v>6.97</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="23">
+      <c r="D4" s="40"/>
+      <c r="E4" s="23">
         <v>0.4</v>
       </c>
-      <c r="E4" s="42"/>
-      <c r="F4" s="17">
+      <c r="F4" s="42"/>
+      <c r="G4" s="17">
         <v>28</v>
       </c>
-      <c r="G4" s="38"/>
-      <c r="H4" s="17">
+      <c r="H4" s="38"/>
+      <c r="I4" s="17">
         <v>24.8</v>
       </c>
-      <c r="I4" s="38"/>
-      <c r="J4" s="27">
+      <c r="J4" s="38"/>
+      <c r="K4" s="27">
         <v>0.21</v>
       </c>
-      <c r="K4" s="45"/>
-      <c r="L4" s="21">
+      <c r="L4" s="45"/>
+      <c r="M4" s="21">
         <v>6.69</v>
       </c>
-      <c r="M4" s="40"/>
-      <c r="N4" s="25">
+      <c r="N4" s="40"/>
+      <c r="O4" s="25">
         <v>135</v>
       </c>
-      <c r="O4" s="39"/>
-      <c r="P4" s="26">
+      <c r="P4" s="39"/>
+      <c r="Q4" s="26">
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:17">
+      <c r="A5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="21">
+      <c r="C5" s="21">
         <v>7.91</v>
       </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="23">
+      <c r="D5" s="40"/>
+      <c r="E5" s="23">
         <v>0.72</v>
       </c>
-      <c r="E5" s="42"/>
-      <c r="F5" s="31">
+      <c r="F5" s="42"/>
+      <c r="G5" s="31">
         <v>66.7</v>
       </c>
-      <c r="G5" s="38"/>
-      <c r="H5" s="17">
+      <c r="H5" s="38"/>
+      <c r="I5" s="17">
         <v>25</v>
       </c>
-      <c r="I5" s="38"/>
-      <c r="J5" s="27">
+      <c r="J5" s="38"/>
+      <c r="K5" s="27">
         <v>0.33500000000000002</v>
       </c>
-      <c r="K5" s="45"/>
-      <c r="L5" s="17">
+      <c r="L5" s="45"/>
+      <c r="M5" s="17">
         <v>15.8</v>
       </c>
-      <c r="M5" s="38"/>
-      <c r="N5" s="17">
+      <c r="N5" s="38"/>
+      <c r="O5" s="17">
         <v>72.099999999999994</v>
       </c>
-      <c r="O5" s="38"/>
-      <c r="P5" s="18">
+      <c r="P5" s="38"/>
+      <c r="Q5" s="18">
         <v>80.099999999999994</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:17">
+      <c r="A6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="21">
+      <c r="C6" s="21">
         <v>3.18</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="23">
+      <c r="D6" s="40"/>
+      <c r="E6" s="23">
         <v>0.38</v>
       </c>
-      <c r="E6" s="42"/>
-      <c r="F6" s="17">
+      <c r="F6" s="42"/>
+      <c r="G6" s="17">
         <v>24.1</v>
       </c>
-      <c r="G6" s="38"/>
-      <c r="H6" s="17">
+      <c r="H6" s="38"/>
+      <c r="I6" s="17">
         <v>15.4</v>
       </c>
-      <c r="I6" s="38"/>
-      <c r="J6" s="23">
+      <c r="J6" s="38"/>
+      <c r="K6" s="23">
         <v>0.27600000000000002</v>
       </c>
-      <c r="K6" s="42"/>
-      <c r="L6" s="21">
+      <c r="L6" s="42"/>
+      <c r="M6" s="21">
         <v>4.79</v>
       </c>
-      <c r="M6" s="40"/>
-      <c r="N6" s="17">
+      <c r="N6" s="40"/>
+      <c r="O6" s="17">
         <v>58.7</v>
       </c>
-      <c r="O6" s="38"/>
-      <c r="P6" s="18">
+      <c r="P6" s="38"/>
+      <c r="Q6" s="18">
         <v>56.1</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:17">
+      <c r="A7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="21">
+      <c r="C7" s="21">
         <v>8.14</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="23">
+      <c r="D7" s="40"/>
+      <c r="E7" s="23">
         <v>0.56999999999999995</v>
       </c>
-      <c r="E7" s="42"/>
-      <c r="F7" s="17">
+      <c r="F7" s="42"/>
+      <c r="G7" s="17">
         <v>34.200000000000003</v>
       </c>
-      <c r="G7" s="38"/>
-      <c r="H7" s="31">
+      <c r="H7" s="38"/>
+      <c r="I7" s="31">
         <v>96.2</v>
       </c>
-      <c r="I7" s="38"/>
-      <c r="J7" s="34">
+      <c r="J7" s="38"/>
+      <c r="K7" s="34">
         <v>1.5489999999999999</v>
       </c>
-      <c r="K7" s="42"/>
-      <c r="L7" s="17">
+      <c r="L7" s="42"/>
+      <c r="M7" s="17">
         <v>19.3</v>
       </c>
-      <c r="M7" s="38"/>
-      <c r="N7" s="35">
+      <c r="N7" s="38"/>
+      <c r="O7" s="35">
         <v>412</v>
       </c>
-      <c r="O7" s="39"/>
-      <c r="P7" s="26">
+      <c r="P7" s="39"/>
+      <c r="Q7" s="26">
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:17">
+      <c r="A8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="21">
+      <c r="C8" s="21">
         <v>6.06</v>
       </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="21">
+      <c r="D8" s="40"/>
+      <c r="E8" s="21">
         <v>0.16</v>
       </c>
-      <c r="E8" s="40"/>
-      <c r="F8" s="17">
+      <c r="F8" s="40"/>
+      <c r="G8" s="17">
         <v>26.2</v>
       </c>
-      <c r="G8" s="38"/>
-      <c r="H8" s="21">
+      <c r="H8" s="38"/>
+      <c r="I8" s="21">
         <v>8.56</v>
       </c>
-      <c r="I8" s="40"/>
-      <c r="J8" s="23">
+      <c r="J8" s="40"/>
+      <c r="K8" s="23">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="K8" s="42"/>
-      <c r="L8" s="21">
+      <c r="L8" s="42"/>
+      <c r="M8" s="21">
         <v>7.2</v>
       </c>
-      <c r="M8" s="40"/>
-      <c r="N8" s="17">
+      <c r="N8" s="40"/>
+      <c r="O8" s="17">
         <v>27.2</v>
       </c>
-      <c r="O8" s="38"/>
-      <c r="P8" s="18">
+      <c r="P8" s="38"/>
+      <c r="Q8" s="18">
         <v>40.6</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:17">
+      <c r="A9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="21">
+      <c r="C9" s="21">
         <v>7.87</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="23">
+      <c r="D9" s="40"/>
+      <c r="E9" s="23">
         <v>0.68</v>
       </c>
-      <c r="E9" s="42"/>
-      <c r="F9" s="17">
+      <c r="F9" s="42"/>
+      <c r="G9" s="17">
         <v>41.4</v>
       </c>
-      <c r="G9" s="38"/>
-      <c r="H9" s="17">
+      <c r="H9" s="38"/>
+      <c r="I9" s="17">
         <v>29.4</v>
       </c>
-      <c r="I9" s="38"/>
-      <c r="J9" s="27">
+      <c r="J9" s="38"/>
+      <c r="K9" s="27">
         <v>0.17399999999999999</v>
       </c>
-      <c r="K9" s="45"/>
-      <c r="L9" s="21">
+      <c r="L9" s="45"/>
+      <c r="M9" s="21">
         <v>20</v>
       </c>
-      <c r="M9" s="40"/>
-      <c r="N9" s="17">
+      <c r="N9" s="40"/>
+      <c r="O9" s="17">
         <v>62.8</v>
       </c>
-      <c r="O9" s="38"/>
-      <c r="P9" s="18">
+      <c r="P9" s="38"/>
+      <c r="Q9" s="18">
         <v>93.8</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:17">
+      <c r="A10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="21">
+      <c r="C10" s="21">
         <v>6.44</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="21">
+      <c r="D10" s="40"/>
+      <c r="E10" s="21">
         <v>0.39</v>
       </c>
-      <c r="E10" s="40"/>
-      <c r="F10" s="17">
+      <c r="F10" s="40"/>
+      <c r="G10" s="17">
         <v>32.6</v>
       </c>
-      <c r="G10" s="38"/>
-      <c r="H10" s="17">
+      <c r="H10" s="38"/>
+      <c r="I10" s="17">
         <v>31.3</v>
       </c>
-      <c r="I10" s="38"/>
-      <c r="J10" s="23">
+      <c r="J10" s="38"/>
+      <c r="K10" s="23">
         <v>0.13</v>
       </c>
-      <c r="K10" s="42"/>
-      <c r="L10" s="17">
+      <c r="L10" s="42"/>
+      <c r="M10" s="17">
         <v>16.2</v>
       </c>
-      <c r="M10" s="38"/>
-      <c r="N10" s="17">
+      <c r="N10" s="38"/>
+      <c r="O10" s="17">
         <v>89.6</v>
       </c>
-      <c r="O10" s="38"/>
-      <c r="P10" s="26">
+      <c r="P10" s="38"/>
+      <c r="Q10" s="26">
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:17">
+      <c r="A11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="17">
+      <c r="C11" s="17">
         <v>11.2</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="23">
+      <c r="D11" s="38"/>
+      <c r="E11" s="23">
         <v>0.92</v>
       </c>
-      <c r="E11" s="42"/>
-      <c r="F11" s="17">
+      <c r="F11" s="42"/>
+      <c r="G11" s="17">
         <v>42.3</v>
       </c>
-      <c r="G11" s="38"/>
-      <c r="H11" s="17">
+      <c r="H11" s="38"/>
+      <c r="I11" s="17">
         <v>33.799999999999997</v>
       </c>
-      <c r="I11" s="38"/>
-      <c r="J11" s="27">
+      <c r="J11" s="38"/>
+      <c r="K11" s="27">
         <v>0.33100000000000002</v>
       </c>
-      <c r="K11" s="45"/>
-      <c r="L11" s="17">
+      <c r="L11" s="45"/>
+      <c r="M11" s="17">
         <v>25.6</v>
       </c>
-      <c r="M11" s="38"/>
-      <c r="N11" s="17">
+      <c r="N11" s="38"/>
+      <c r="O11" s="17">
         <v>84.9</v>
       </c>
-      <c r="O11" s="38"/>
-      <c r="P11" s="26">
+      <c r="P11" s="38"/>
+      <c r="Q11" s="26">
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
-      <c r="A12" s="32" t="s">
+    <row r="12" spans="1:17">
+      <c r="A12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="17">
+      <c r="C12" s="17">
         <v>11.4</v>
       </c>
-      <c r="C12" s="38"/>
-      <c r="D12" s="21">
+      <c r="D12" s="38"/>
+      <c r="E12" s="21">
         <v>0.68</v>
       </c>
-      <c r="E12" s="40"/>
-      <c r="F12" s="17">
+      <c r="F12" s="40"/>
+      <c r="G12" s="17">
         <v>49.9</v>
       </c>
-      <c r="G12" s="38"/>
-      <c r="H12" s="33">
+      <c r="H12" s="38"/>
+      <c r="I12" s="33">
         <v>103</v>
       </c>
-      <c r="I12" s="39"/>
-      <c r="J12" s="23">
+      <c r="J12" s="39"/>
+      <c r="K12" s="23">
         <v>0.37</v>
       </c>
-      <c r="K12" s="42"/>
-      <c r="L12" s="17">
+      <c r="L12" s="42"/>
+      <c r="M12" s="17">
         <v>24.6</v>
       </c>
-      <c r="M12" s="38"/>
-      <c r="N12" s="35">
+      <c r="N12" s="38"/>
+      <c r="O12" s="35">
         <v>491</v>
       </c>
-      <c r="O12" s="39"/>
-      <c r="P12" s="36">
+      <c r="P12" s="39"/>
+      <c r="Q12" s="36">
         <v>460</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
-      <c r="A13" s="32" t="s">
+    <row r="13" spans="1:17">
+      <c r="A13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="21">
+      <c r="C13" s="21">
         <v>8.3800000000000008</v>
       </c>
-      <c r="C13" s="40"/>
-      <c r="D13" s="23">
+      <c r="D13" s="40"/>
+      <c r="E13" s="23">
         <v>0.67</v>
       </c>
-      <c r="E13" s="42"/>
-      <c r="F13" s="17">
+      <c r="F13" s="42"/>
+      <c r="G13" s="17">
         <v>45.8</v>
       </c>
-      <c r="G13" s="38"/>
-      <c r="H13" s="17">
+      <c r="H13" s="38"/>
+      <c r="I13" s="17">
         <v>25.7</v>
       </c>
-      <c r="I13" s="38"/>
-      <c r="J13" s="27">
+      <c r="J13" s="38"/>
+      <c r="K13" s="27">
         <v>0.27800000000000002</v>
       </c>
-      <c r="K13" s="45"/>
-      <c r="L13" s="17">
+      <c r="L13" s="45"/>
+      <c r="M13" s="17">
         <v>23.1</v>
       </c>
-      <c r="M13" s="38"/>
-      <c r="N13" s="17">
+      <c r="N13" s="38"/>
+      <c r="O13" s="17">
         <v>93.5</v>
       </c>
-      <c r="O13" s="38"/>
-      <c r="P13" s="26">
+      <c r="P13" s="38"/>
+      <c r="Q13" s="26">
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
-      <c r="A14" s="32" t="s">
+    <row r="14" spans="1:17">
+      <c r="A14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="21">
+      <c r="C14" s="21">
         <v>5.8</v>
       </c>
-      <c r="C14" s="40"/>
-      <c r="D14" s="23">
+      <c r="D14" s="40"/>
+      <c r="E14" s="23">
         <v>0.47</v>
       </c>
-      <c r="E14" s="42"/>
-      <c r="F14" s="17">
+      <c r="F14" s="42"/>
+      <c r="G14" s="17">
         <v>40.700000000000003</v>
       </c>
-      <c r="G14" s="38"/>
-      <c r="H14" s="17">
+      <c r="H14" s="38"/>
+      <c r="I14" s="17">
         <v>43.6</v>
       </c>
-      <c r="I14" s="38"/>
-      <c r="J14" s="27">
+      <c r="J14" s="38"/>
+      <c r="K14" s="27">
         <v>0.51800000000000002</v>
       </c>
-      <c r="K14" s="45"/>
-      <c r="L14" s="17">
+      <c r="L14" s="45"/>
+      <c r="M14" s="17">
         <v>13.6</v>
       </c>
-      <c r="M14" s="38"/>
-      <c r="N14" s="25">
+      <c r="N14" s="38"/>
+      <c r="O14" s="25">
         <v>128</v>
       </c>
-      <c r="O14" s="39"/>
-      <c r="P14" s="26">
+      <c r="P14" s="39"/>
+      <c r="Q14" s="26">
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="32" t="s">
+    <row r="15" spans="1:17">
+      <c r="A15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="21">
+      <c r="C15" s="21">
         <v>7.46</v>
       </c>
-      <c r="C15" s="40"/>
-      <c r="D15" s="23">
+      <c r="D15" s="40"/>
+      <c r="E15" s="23">
         <v>0.46</v>
       </c>
-      <c r="E15" s="42"/>
-      <c r="F15" s="17">
+      <c r="F15" s="42"/>
+      <c r="G15" s="17">
         <v>38.6</v>
       </c>
-      <c r="G15" s="38"/>
-      <c r="H15" s="17">
+      <c r="H15" s="38"/>
+      <c r="I15" s="17">
         <v>18.7</v>
       </c>
-      <c r="I15" s="38"/>
-      <c r="J15" s="23">
+      <c r="J15" s="38"/>
+      <c r="K15" s="23">
         <v>0.12</v>
       </c>
-      <c r="K15" s="42"/>
-      <c r="L15" s="17">
+      <c r="L15" s="42"/>
+      <c r="M15" s="17">
         <v>20.6</v>
       </c>
-      <c r="M15" s="38"/>
-      <c r="N15" s="17">
+      <c r="N15" s="38"/>
+      <c r="O15" s="17">
         <v>39.700000000000003</v>
       </c>
-      <c r="O15" s="38"/>
-      <c r="P15" s="18">
+      <c r="P15" s="38"/>
+      <c r="Q15" s="18">
         <v>65.2</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
-      <c r="A16" s="32" t="s">
+    <row r="16" spans="1:17">
+      <c r="A16" t="s">
+        <v>108</v>
+      </c>
+      <c r="B16" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="22">
+      <c r="C16" s="22">
         <v>4.53</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="24">
+      <c r="D16" s="41"/>
+      <c r="E16" s="24">
         <v>0.44</v>
       </c>
-      <c r="E16" s="43"/>
-      <c r="F16" s="19">
+      <c r="F16" s="43"/>
+      <c r="G16" s="19">
         <v>25.3</v>
       </c>
-      <c r="G16" s="44"/>
-      <c r="H16" s="22">
+      <c r="H16" s="44"/>
+      <c r="I16" s="22">
         <v>9.91</v>
       </c>
-      <c r="I16" s="41"/>
-      <c r="J16" s="30">
+      <c r="J16" s="41"/>
+      <c r="K16" s="30">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="K16" s="46"/>
-      <c r="L16" s="22">
+      <c r="L16" s="46"/>
+      <c r="M16" s="22">
         <v>7.99</v>
       </c>
-      <c r="M16" s="41"/>
-      <c r="N16" s="19">
+      <c r="N16" s="41"/>
+      <c r="O16" s="19">
         <v>50.4</v>
       </c>
-      <c r="O16" s="44"/>
-      <c r="P16" s="20">
+      <c r="P16" s="44"/>
+      <c r="Q16" s="20">
         <v>64.7</v>
       </c>
     </row>
-    <row r="17" spans="1:16" s="75" customFormat="1" ht="66" customHeight="1">
-      <c r="A17" s="118" t="s">
+    <row r="17" spans="2:17" s="75" customFormat="1" ht="66" customHeight="1">
+      <c r="B17" s="130" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="119"/>
-      <c r="C17" s="119"/>
-      <c r="D17" s="119"/>
-      <c r="E17" s="119"/>
-      <c r="F17" s="119"/>
-      <c r="G17" s="119"/>
-      <c r="H17" s="119"/>
-      <c r="I17" s="119"/>
-      <c r="J17" s="119"/>
-      <c r="K17" s="119"/>
-      <c r="L17" s="119"/>
-      <c r="M17" s="119"/>
-      <c r="N17" s="119"/>
-      <c r="O17" s="119"/>
-      <c r="P17" s="120"/>
-    </row>
-    <row r="18" spans="1:16" s="97" customFormat="1">
-      <c r="A18" s="121" t="s">
+      <c r="C17" s="131"/>
+      <c r="D17" s="131"/>
+      <c r="E17" s="131"/>
+      <c r="F17" s="131"/>
+      <c r="G17" s="131"/>
+      <c r="H17" s="131"/>
+      <c r="I17" s="131"/>
+      <c r="J17" s="131"/>
+      <c r="K17" s="131"/>
+      <c r="L17" s="131"/>
+      <c r="M17" s="131"/>
+      <c r="N17" s="131"/>
+      <c r="O17" s="131"/>
+      <c r="P17" s="131"/>
+      <c r="Q17" s="132"/>
+    </row>
+    <row r="18" spans="2:17" s="97" customFormat="1">
+      <c r="B18" s="128" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="122"/>
-      <c r="C18" s="121" t="s">
+      <c r="C18" s="129"/>
+      <c r="D18" s="128" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="122"/>
-      <c r="E18" s="121" t="s">
+      <c r="E18" s="129"/>
+      <c r="F18" s="128" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="122"/>
-      <c r="G18" s="121" t="s">
+      <c r="G18" s="129"/>
+      <c r="H18" s="128" t="s">
         <v>29</v>
       </c>
-      <c r="H18" s="122"/>
-      <c r="I18" s="121" t="s">
+      <c r="I18" s="129"/>
+      <c r="J18" s="128" t="s">
         <v>30</v>
       </c>
-      <c r="J18" s="122"/>
-      <c r="K18" s="121" t="s">
+      <c r="K18" s="129"/>
+      <c r="L18" s="128" t="s">
         <v>33</v>
       </c>
-      <c r="L18" s="122"/>
-      <c r="M18" s="121" t="s">
+      <c r="M18" s="129"/>
+      <c r="N18" s="128" t="s">
         <v>31</v>
       </c>
-      <c r="N18" s="122"/>
-      <c r="O18" s="121" t="s">
+      <c r="O18" s="129"/>
+      <c r="P18" s="128" t="s">
         <v>32</v>
       </c>
-      <c r="P18" s="122"/>
-    </row>
-    <row r="19" spans="1:16">
-      <c r="A19" s="8" t="s">
+      <c r="Q18" s="129"/>
+    </row>
+    <row r="19" spans="2:17">
+      <c r="B19" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="47">
+      <c r="C19" s="47">
         <v>3.18</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="D19" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="47">
+      <c r="E19" s="47">
         <v>0.16</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="F19" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F19" s="48">
+      <c r="G19" s="48">
         <v>24.1</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="H19" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H19" s="47">
+      <c r="I19" s="47">
         <v>8.56</v>
       </c>
-      <c r="I19" s="8" t="s">
+      <c r="J19" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J19" s="49">
+      <c r="K19" s="49">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="K19" s="8" t="s">
+      <c r="L19" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="L19" s="47">
+      <c r="M19" s="47">
         <v>4.79</v>
       </c>
-      <c r="M19" s="8" t="s">
+      <c r="N19" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="N19" s="48">
+      <c r="O19" s="48">
         <v>27.2</v>
       </c>
-      <c r="O19" s="8" t="s">
+      <c r="P19" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="P19" s="83">
+      <c r="Q19" s="83">
         <v>40.6</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
-      <c r="A20" s="32" t="s">
+    <row r="20" spans="2:17">
+      <c r="B20" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="47">
+      <c r="C20" s="47">
         <v>4.53</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="49">
+      <c r="E20" s="49">
         <v>0.38</v>
       </c>
-      <c r="E20" s="32" t="s">
+      <c r="F20" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="48">
+      <c r="G20" s="48">
         <v>25.3</v>
       </c>
-      <c r="G20" s="32" t="s">
+      <c r="H20" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="H20" s="47">
+      <c r="I20" s="47">
         <v>9.91</v>
       </c>
-      <c r="I20" s="4" t="s">
+      <c r="J20" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="J20" s="49">
+      <c r="K20" s="49">
         <v>0.08</v>
       </c>
-      <c r="K20" s="4" t="s">
+      <c r="L20" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="L20" s="47">
+      <c r="M20" s="47">
         <v>6.69</v>
       </c>
-      <c r="M20" s="4" t="s">
+      <c r="N20" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="N20" s="48">
+      <c r="O20" s="48">
         <v>34.1</v>
       </c>
-      <c r="O20" s="4" t="s">
+      <c r="P20" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="P20" s="83">
+      <c r="Q20" s="83">
         <v>56.1</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
-      <c r="A21" s="32" t="s">
+    <row r="21" spans="2:17">
+      <c r="B21" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="47">
+      <c r="C21" s="47">
         <v>5.8</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="D21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="47">
+      <c r="E21" s="47">
         <v>0.39</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="F21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="48">
+      <c r="G21" s="48">
         <v>26.2</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="H21" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H21" s="48">
+      <c r="I21" s="48">
         <v>15.4</v>
       </c>
-      <c r="I21" s="32" t="s">
+      <c r="J21" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="J21" s="51">
+      <c r="K21" s="51">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="K21" s="4" t="s">
+      <c r="L21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="L21" s="47">
+      <c r="M21" s="47">
         <v>7.2</v>
       </c>
-      <c r="M21" s="32" t="s">
+      <c r="N21" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="N21" s="48">
+      <c r="O21" s="48">
         <v>39.700000000000003</v>
       </c>
-      <c r="O21" s="32" t="s">
+      <c r="P21" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="P21" s="83">
+      <c r="Q21" s="83">
         <v>64.7</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="2:17">
+      <c r="B22" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="47">
+      <c r="C22" s="47">
         <v>6.06</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="49">
+      <c r="E22" s="49">
         <v>0.4</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="F22" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F22" s="48">
+      <c r="G22" s="48">
         <v>28</v>
       </c>
-      <c r="G22" s="32" t="s">
+      <c r="H22" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="H22" s="48">
+      <c r="I22" s="48">
         <v>18.7</v>
       </c>
-      <c r="I22" s="8" t="s">
+      <c r="J22" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="J22" s="49">
+      <c r="K22" s="49">
         <v>0.12</v>
       </c>
-      <c r="K22" s="32" t="s">
+      <c r="L22" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="L22" s="47">
+      <c r="M22" s="47">
         <v>7.99</v>
       </c>
-      <c r="M22" s="32" t="s">
+      <c r="N22" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="N22" s="48">
+      <c r="O22" s="48">
         <v>50.4</v>
       </c>
-      <c r="O22" s="32" t="s">
+      <c r="P22" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="P22" s="83">
+      <c r="Q22" s="83">
         <v>65.2</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
-      <c r="A23" s="8" t="s">
+    <row r="23" spans="2:17">
+      <c r="B23" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="47">
+      <c r="C23" s="47">
         <v>6.27</v>
       </c>
-      <c r="C23" s="32" t="s">
+      <c r="D23" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="49">
+      <c r="E23" s="49">
         <v>0.44</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="F23" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F23" s="48">
+      <c r="G23" s="48">
         <v>32.6</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="H23" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H23" s="48">
+      <c r="I23" s="48">
         <v>20.7</v>
       </c>
-      <c r="I23" s="32" t="s">
+      <c r="J23" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="J23" s="49">
+      <c r="K23" s="49">
         <v>0.12</v>
       </c>
-      <c r="K23" s="32" t="s">
+      <c r="L23" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="L23" s="48">
+      <c r="M23" s="48">
         <v>13.6</v>
       </c>
-      <c r="M23" s="4" t="s">
+      <c r="N23" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="N23" s="48">
+      <c r="O23" s="48">
         <v>58.7</v>
       </c>
-      <c r="O23" s="4" t="s">
+      <c r="P23" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="P23" s="83">
+      <c r="Q23" s="83">
         <v>80.099999999999994</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
-      <c r="A24" s="4" t="s">
+    <row r="24" spans="2:17">
+      <c r="B24" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="47">
+      <c r="C24" s="47">
         <v>6.33</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="D24" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D24" s="47">
+      <c r="E24" s="47">
         <v>0.46</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="F24" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="48">
+      <c r="G24" s="48">
         <v>34.200000000000003</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="H24" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H24" s="48">
+      <c r="I24" s="48">
         <v>24.8</v>
       </c>
-      <c r="I24" s="4" t="s">
+      <c r="J24" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J24" s="49">
+      <c r="K24" s="49">
         <v>0.13</v>
       </c>
-      <c r="K24" s="8" t="s">
+      <c r="L24" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="L24" s="48">
+      <c r="M24" s="48">
         <v>13.7</v>
       </c>
-      <c r="M24" s="4" t="s">
+      <c r="N24" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N24" s="48">
+      <c r="O24" s="48">
         <v>62.8</v>
       </c>
-      <c r="O24" s="4" t="s">
+      <c r="P24" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="P24" s="83">
+      <c r="Q24" s="83">
         <v>93.2</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
-      <c r="A25" s="4" t="s">
+    <row r="25" spans="2:17">
+      <c r="B25" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="47">
+      <c r="C25" s="47">
         <v>6.44</v>
       </c>
-      <c r="C25" s="32" t="s">
+      <c r="D25" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="49">
+      <c r="E25" s="49">
         <v>0.46</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="F25" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="F25" s="48">
+      <c r="G25" s="48">
         <v>36.200000000000003</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="H25" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H25" s="48">
+      <c r="I25" s="48">
         <v>25</v>
       </c>
-      <c r="I25" s="4" t="s">
+      <c r="J25" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J25" s="51">
+      <c r="K25" s="51">
         <v>0.17399999999999999</v>
       </c>
-      <c r="K25" s="4" t="s">
+      <c r="L25" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="L25" s="48">
+      <c r="M25" s="48">
         <v>15.8</v>
       </c>
-      <c r="M25" s="4" t="s">
+      <c r="N25" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="N25" s="48">
+      <c r="O25" s="48">
         <v>72.099999999999994</v>
       </c>
-      <c r="O25" s="4" t="s">
+      <c r="P25" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="P25" s="83">
+      <c r="Q25" s="83">
         <v>93.8</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
-      <c r="A26" s="4" t="s">
+    <row r="26" spans="2:17">
+      <c r="B26" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="47">
+      <c r="C26" s="47">
         <v>6.97</v>
       </c>
-      <c r="C26" s="32" t="s">
+      <c r="D26" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="49">
+      <c r="E26" s="49">
         <v>0.47</v>
       </c>
-      <c r="E26" s="32" t="s">
+      <c r="F26" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="F26" s="48">
+      <c r="G26" s="48">
         <v>38.6</v>
       </c>
-      <c r="G26" s="32" t="s">
+      <c r="H26" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="H26" s="48">
+      <c r="I26" s="48">
         <v>25.7</v>
       </c>
-      <c r="I26" s="4" t="s">
+      <c r="J26" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="J26" s="51">
+      <c r="K26" s="51">
         <v>0.21</v>
       </c>
-      <c r="K26" s="4" t="s">
+      <c r="L26" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L26" s="48">
+      <c r="M26" s="48">
         <v>16.2</v>
       </c>
-      <c r="M26" s="4" t="s">
+      <c r="N26" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="N26" s="48">
+      <c r="O26" s="48">
         <v>84.9</v>
       </c>
-      <c r="O26" s="32" t="s">
+      <c r="P26" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="P26" s="84">
+      <c r="Q26" s="84">
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
-      <c r="A27" s="32" t="s">
+    <row r="27" spans="2:17">
+      <c r="B27" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="47">
+      <c r="C27" s="47">
         <v>7.46</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D27" s="49">
+      <c r="E27" s="49">
         <v>0.56999999999999995</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="F27" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F27" s="48">
+      <c r="G27" s="48">
         <v>39.6</v>
       </c>
-      <c r="G27" s="4" t="s">
+      <c r="H27" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H27" s="48">
+      <c r="I27" s="48">
         <v>29.4</v>
       </c>
-      <c r="I27" s="4" t="s">
+      <c r="J27" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J27" s="49">
+      <c r="K27" s="49">
         <v>0.27600000000000002</v>
       </c>
-      <c r="K27" s="4" t="s">
+      <c r="L27" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="L27" s="48">
+      <c r="M27" s="48">
         <v>16.5</v>
       </c>
-      <c r="M27" s="8" t="s">
+      <c r="N27" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="N27" s="48">
+      <c r="O27" s="48">
         <v>89.6</v>
       </c>
-      <c r="O27" s="8" t="s">
+      <c r="P27" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="P27" s="84">
+      <c r="Q27" s="84">
         <v>115</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
-      <c r="A28" s="4" t="s">
+    <row r="28" spans="2:17">
+      <c r="B28" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="47">
+      <c r="C28" s="47">
         <v>7.87</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="D28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D28" s="47">
+      <c r="E28" s="47">
         <v>0.64</v>
       </c>
-      <c r="E28" s="32" t="s">
+      <c r="F28" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="F28" s="48">
+      <c r="G28" s="48">
         <v>40.700000000000003</v>
       </c>
-      <c r="G28" s="8" t="s">
+      <c r="H28" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="H28" s="48">
+      <c r="I28" s="48">
         <v>29.5</v>
       </c>
-      <c r="I28" s="32" t="s">
+      <c r="J28" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="J28" s="51">
+      <c r="K28" s="51">
         <v>0.27800000000000002</v>
       </c>
-      <c r="K28" s="4" t="s">
+      <c r="L28" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="L28" s="48">
+      <c r="M28" s="48">
         <v>19.3</v>
       </c>
-      <c r="M28" s="4" t="s">
+      <c r="N28" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="N28" s="48">
+      <c r="O28" s="48">
         <v>89.6</v>
       </c>
-      <c r="O28" s="32" t="s">
+      <c r="P28" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="P28" s="84">
+      <c r="Q28" s="84">
         <v>117</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
-      <c r="A29" s="4" t="s">
+    <row r="29" spans="2:17">
+      <c r="B29" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="47">
+      <c r="C29" s="47">
         <v>7.91</v>
       </c>
-      <c r="C29" s="32" t="s">
+      <c r="D29" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="D29" s="49">
+      <c r="E29" s="49">
         <v>0.67</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="F29" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F29" s="48">
+      <c r="G29" s="48">
         <v>41.4</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="H29" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H29" s="48">
+      <c r="I29" s="48">
         <v>31.3</v>
       </c>
-      <c r="I29" s="4" t="s">
+      <c r="J29" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="J29" s="51">
+      <c r="K29" s="51">
         <v>0.33100000000000002</v>
       </c>
-      <c r="K29" s="4" t="s">
+      <c r="L29" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L29" s="47">
+      <c r="M29" s="47">
         <v>20</v>
       </c>
-      <c r="M29" s="32" t="s">
+      <c r="N29" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="N29" s="48">
+      <c r="O29" s="48">
         <v>93.5</v>
       </c>
-      <c r="O29" s="4" t="s">
+      <c r="P29" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="P29" s="84">
+      <c r="Q29" s="84">
         <v>119</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
-      <c r="A30" s="4" t="s">
+    <row r="30" spans="2:17">
+      <c r="B30" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B30" s="47">
+      <c r="C30" s="47">
         <v>8.14</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="D30" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="49">
+      <c r="E30" s="49">
         <v>0.68</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="F30" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F30" s="48">
+      <c r="G30" s="48">
         <v>42.3</v>
       </c>
-      <c r="G30" s="4" t="s">
+      <c r="H30" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="H30" s="48">
+      <c r="I30" s="48">
         <v>33.799999999999997</v>
       </c>
-      <c r="I30" s="4" t="s">
+      <c r="J30" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J30" s="51">
+      <c r="K30" s="51">
         <v>0.33500000000000002</v>
       </c>
-      <c r="K30" s="32" t="s">
+      <c r="L30" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="L30" s="48">
+      <c r="M30" s="48">
         <v>20.6</v>
       </c>
-      <c r="M30" s="32" t="s">
+      <c r="N30" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="N30" s="52">
+      <c r="O30" s="52">
         <v>128</v>
       </c>
-      <c r="O30" s="4" t="s">
+      <c r="P30" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="P30" s="84">
+      <c r="Q30" s="84">
         <v>123</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
-      <c r="A31" s="32" t="s">
+    <row r="31" spans="2:17">
+      <c r="B31" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="47">
+      <c r="C31" s="47">
         <v>8.3800000000000008</v>
       </c>
-      <c r="C31" s="32" t="s">
+      <c r="D31" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="D31" s="47">
+      <c r="E31" s="47">
         <v>0.68</v>
       </c>
-      <c r="E31" s="32" t="s">
+      <c r="F31" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="F31" s="48">
+      <c r="G31" s="48">
         <v>45.8</v>
       </c>
-      <c r="G31" s="32" t="s">
+      <c r="H31" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="H31" s="48">
+      <c r="I31" s="48">
         <v>43.6</v>
       </c>
-      <c r="I31" s="32" t="s">
+      <c r="J31" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="J31" s="49">
+      <c r="K31" s="49">
         <v>0.37</v>
       </c>
-      <c r="K31" s="32" t="s">
+      <c r="L31" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="L31" s="48">
+      <c r="M31" s="48">
         <v>23.1</v>
       </c>
-      <c r="M31" s="4" t="s">
+      <c r="N31" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="N31" s="52">
+      <c r="O31" s="52">
         <v>135</v>
       </c>
-      <c r="O31" s="4" t="s">
+      <c r="P31" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="P31" s="84">
+      <c r="Q31" s="84">
         <v>143</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
-      <c r="A32" s="4" t="s">
+    <row r="32" spans="2:17">
+      <c r="B32" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="48">
+      <c r="C32" s="48">
         <v>11.2</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D32" s="49">
+      <c r="E32" s="49">
         <v>0.72</v>
       </c>
-      <c r="E32" s="32" t="s">
+      <c r="F32" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="F32" s="48">
+      <c r="G32" s="48">
         <v>49.9</v>
       </c>
-      <c r="G32" s="4" t="s">
+      <c r="H32" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H32" s="50">
+      <c r="I32" s="50">
         <v>96.2</v>
       </c>
-      <c r="I32" s="32" t="s">
+      <c r="J32" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="J32" s="51">
+      <c r="K32" s="51">
         <v>0.51800000000000002</v>
       </c>
-      <c r="K32" s="32" t="s">
+      <c r="L32" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="L32" s="48">
+      <c r="M32" s="48">
         <v>24.6</v>
       </c>
-      <c r="M32" s="4" t="s">
+      <c r="N32" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N32" s="53">
+      <c r="O32" s="53">
         <v>412</v>
       </c>
-      <c r="O32" s="4" t="s">
+      <c r="P32" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="P32" s="84">
+      <c r="Q32" s="84">
         <v>144</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
-      <c r="A33" s="32" t="s">
+    <row r="33" spans="2:17">
+      <c r="B33" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B33" s="85">
+      <c r="C33" s="85">
         <v>11.4</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="D33" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D33" s="86">
+      <c r="E33" s="86">
         <v>0.92</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="F33" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F33" s="87">
+      <c r="G33" s="87">
         <v>66.7</v>
       </c>
-      <c r="G33" s="32" t="s">
+      <c r="H33" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="H33" s="88">
+      <c r="I33" s="88">
         <v>103</v>
       </c>
-      <c r="I33" s="4" t="s">
+      <c r="J33" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J33" s="89">
+      <c r="K33" s="89">
         <v>1.5489999999999999</v>
       </c>
-      <c r="K33" s="4" t="s">
+      <c r="L33" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L33" s="85">
+      <c r="M33" s="85">
         <v>25.6</v>
       </c>
-      <c r="M33" s="32" t="s">
+      <c r="N33" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="N33" s="90">
+      <c r="O33" s="90">
         <v>491</v>
       </c>
-      <c r="O33" s="32" t="s">
+      <c r="P33" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="P33" s="91">
+      <c r="Q33" s="91">
         <v>460</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="A17:P17"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="P18:Q18"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="B17:Q17"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B2:B16">
+  <phoneticPr fontId="4" type="noConversion"/>
+  <conditionalFormatting sqref="C2:C16">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -6510,7 +6607,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D16">
+  <conditionalFormatting sqref="E2:E16">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -6522,7 +6619,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F16">
+  <conditionalFormatting sqref="G2:G16">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -6534,7 +6631,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H16">
+  <conditionalFormatting sqref="I2:I16">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -6546,7 +6643,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J16">
+  <conditionalFormatting sqref="K2:K16">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -6558,7 +6655,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L16">
+  <conditionalFormatting sqref="M2:M16">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -6570,7 +6667,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N16">
+  <conditionalFormatting sqref="O2:O16">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -6582,7 +6679,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P2:P16">
+  <conditionalFormatting sqref="Q2:Q16">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -6607,7 +6704,7 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="14.625" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
@@ -6620,14 +6717,14 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1"/>
-      <c r="B1" s="123" t="s">
+      <c r="B1" s="133" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="124" t="s">
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="134" t="s">
         <v>53</v>
       </c>
     </row>
@@ -6650,7 +6747,7 @@
       <c r="F2" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="124"/>
+      <c r="G2" s="134"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="13" t="s">

</xml_diff>